<commit_message>
Xsd changes region id invoice added ie037 17 nov2023 (#180)
* un-deprecate DK2008 (#220)

* XSD Changes Invoice Region Added IE037 (#221)

* InvoiceAmount mandatory for B1, B2, B4 and C1 Supplementary

* RegionID removed from B1, B2, B3, B4, C1 and C1 Supplementary

* Updated version numbers for changed XSDs

* Aligning version number

* Add IE037 XSD

---------

Co-authored-by: emha <emha@netcompany.com>

* Update DMS_C1_Amendment_Correction_v1.27.xsd

* Update schemaLocation in IE037 (#222)

* Update schemaLocation in IE037

* Update changelog.md

---------

Co-authored-by: emha <emha@netcompany.com>
Co-authored-by: Erik Rolander <nc-erro@github.com>
Co-authored-by: nc-erro <137885287+nc-erro@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Onboarding Documents/Error and warning codes.xlsx
+++ b/Onboarding Documents/Error and warning codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netcompany-my.sharepoint.com/personal/albt_netcompany_com/Documents/Dokumenter/GitHub/dms-public-private/Onboarding Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albt\OneDrive - Netcompany\Dokumenter\GitHub\dms-public-private\Onboarding Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{5210483F-ED55-4B6D-9C2F-A8B1A45F6BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4DFBEC8-F427-426A-A1FE-63C275E34DE4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E971EA4-E18A-4771-9616-E28F4F81B53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B85A02ED-9ABC-4F63-82FC-39E5924E62E4}"/>
+    <workbookView xWindow="31320" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{B85A02ED-9ABC-4F63-82FC-39E5924E62E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="1011">
   <si>
     <t>Error code</t>
   </si>
@@ -3066,6 +3066,9 @@
   </si>
   <si>
     <t>When an IE590 is received and it refers to an IE547 (this is checked outside this rule), then the IE547 must exist in the solution</t>
+  </si>
+  <si>
+    <t>DKW2008</t>
   </si>
 </sst>
 </file>
@@ -3759,7 +3762,7 @@
     <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3917,9 +3920,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3964,6 +3964,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -4323,8 +4347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C124F3A-70A1-4C39-B88D-70E9954F3B3C}">
   <dimension ref="A1:K348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4677,21 +4701,21 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="66" t="s">
         <v>1006</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="68" t="s">
+      <c r="B38" s="66"/>
+      <c r="C38" s="67" t="s">
         <v>1007</v>
       </c>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -4772,7 +4796,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>98</v>
       </c>
@@ -4898,7 +4922,7 @@
       </c>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>127</v>
       </c>
@@ -4912,7 +4936,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>131</v>
       </c>
@@ -5046,7 +5070,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>165</v>
       </c>
@@ -5584,7 +5608,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="113" spans="1:4" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>295</v>
       </c>
@@ -5610,7 +5634,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="115" spans="1:4" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>302</v>
       </c>
@@ -5664,7 +5688,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="1:4" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>317</v>
       </c>
@@ -5720,7 +5744,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="123" spans="1:4" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>333</v>
       </c>
@@ -5906,7 +5930,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>381</v>
       </c>
@@ -5976,7 +6000,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
         <v>398</v>
       </c>
@@ -6048,7 +6072,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="150" spans="1:4" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>412</v>
       </c>
@@ -6212,7 +6236,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="164" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>449</v>
       </c>
@@ -6249,7 +6273,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="63" t="s">
+      <c r="A167" s="62" t="s">
         <v>985</v>
       </c>
       <c r="B167" s="9"/>
@@ -6273,7 +6297,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A169" s="63" t="s">
+      <c r="A169" s="62" t="s">
         <v>987</v>
       </c>
       <c r="B169" s="9"/>
@@ -6297,10 +6321,10 @@
       </c>
     </row>
     <row r="171" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="62" t="s">
+      <c r="A171" s="61" t="s">
         <v>989</v>
       </c>
-      <c r="B171" s="60"/>
+      <c r="B171" s="59"/>
       <c r="C171" s="34" t="s">
         <v>994</v>
       </c>
@@ -6309,26 +6333,26 @@
       </c>
     </row>
     <row r="172" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A172" s="65" t="s">
+      <c r="A172" s="64" t="s">
         <v>1000</v>
       </c>
       <c r="B172" s="7"/>
-      <c r="C172" s="64" t="s">
+      <c r="C172" s="63" t="s">
         <v>1001</v>
       </c>
-      <c r="D172" s="64" t="s">
+      <c r="D172" s="63" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A173" s="61" t="s">
+      <c r="A173" s="60" t="s">
         <v>1003</v>
       </c>
       <c r="B173" s="9"/>
-      <c r="C173" s="66" t="s">
+      <c r="C173" s="65" t="s">
         <v>1004</v>
       </c>
-      <c r="D173" s="66" t="s">
+      <c r="D173" s="65" t="s">
         <v>1005</v>
       </c>
     </row>
@@ -6390,11 +6414,11 @@
       <c r="A178" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="B178" s="32"/>
-      <c r="C178" s="39" t="s">
+      <c r="B178" s="68"/>
+      <c r="C178" s="70" t="s">
         <v>470</v>
       </c>
-      <c r="D178" s="34" t="s">
+      <c r="D178" s="69" t="s">
         <v>471</v>
       </c>
     </row>
@@ -6416,13 +6440,13 @@
       <c r="A180" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B180" s="32" t="s">
+      <c r="B180" s="68" t="s">
         <v>477</v>
       </c>
-      <c r="C180" s="39" t="s">
+      <c r="C180" s="70" t="s">
         <v>478</v>
       </c>
-      <c r="D180" s="34" t="s">
+      <c r="D180" s="69" t="s">
         <v>479</v>
       </c>
     </row>
@@ -6444,13 +6468,13 @@
       <c r="A182" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="B182" s="38" t="s">
-        <v>977</v>
-      </c>
-      <c r="C182" s="51" t="s">
+      <c r="B182" s="32" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C182" s="69" t="s">
         <v>485</v>
       </c>
-      <c r="D182" s="51" t="s">
+      <c r="D182" s="69" t="s">
         <v>486</v>
       </c>
     </row>
@@ -6472,13 +6496,13 @@
       <c r="A184" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="B184" s="32" t="s">
+      <c r="B184" s="68" t="s">
         <v>492</v>
       </c>
-      <c r="C184" s="34" t="s">
+      <c r="C184" s="69" t="s">
         <v>493</v>
       </c>
-      <c r="D184" s="34" t="s">
+      <c r="D184" s="69" t="s">
         <v>494</v>
       </c>
     </row>
@@ -6500,13 +6524,13 @@
       <c r="A186" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="B186" s="32" t="s">
+      <c r="B186" s="68" t="s">
         <v>500</v>
       </c>
-      <c r="C186" s="37" t="s">
+      <c r="C186" s="71" t="s">
         <v>501</v>
       </c>
-      <c r="D186" s="34" t="s">
+      <c r="D186" s="69" t="s">
         <v>502</v>
       </c>
     </row>
@@ -6514,7 +6538,7 @@
       <c r="A187" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="B187" s="57"/>
+      <c r="B187" s="56"/>
       <c r="C187" s="37" t="s">
         <v>504</v>
       </c>
@@ -6526,11 +6550,11 @@
       <c r="A188" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="B188" s="57"/>
-      <c r="C188" s="37" t="s">
+      <c r="B188" s="72"/>
+      <c r="C188" s="71" t="s">
         <v>507</v>
       </c>
-      <c r="D188" s="34" t="s">
+      <c r="D188" s="69" t="s">
         <v>508</v>
       </c>
     </row>
@@ -6538,7 +6562,7 @@
       <c r="A189" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B189" s="57"/>
+      <c r="B189" s="56"/>
       <c r="C189" s="37" t="s">
         <v>510</v>
       </c>
@@ -6550,11 +6574,11 @@
       <c r="A190" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="B190" s="57"/>
-      <c r="C190" s="52" t="s">
+      <c r="B190" s="72"/>
+      <c r="C190" s="73" t="s">
         <v>513</v>
       </c>
-      <c r="D190" s="34" t="s">
+      <c r="D190" s="69" t="s">
         <v>514</v>
       </c>
     </row>
@@ -6562,7 +6586,7 @@
       <c r="A191" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="B191" s="57"/>
+      <c r="B191" s="56"/>
       <c r="C191" s="52" t="s">
         <v>516</v>
       </c>
@@ -6574,11 +6598,11 @@
       <c r="A192" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="B192" s="57"/>
-      <c r="C192" s="52" t="s">
+      <c r="B192" s="72"/>
+      <c r="C192" s="73" t="s">
         <v>519</v>
       </c>
-      <c r="D192" s="34" t="s">
+      <c r="D192" s="69" t="s">
         <v>520</v>
       </c>
     </row>
@@ -6586,7 +6610,7 @@
       <c r="A193" s="9" t="s">
         <v>521</v>
       </c>
-      <c r="B193" s="57" t="s">
+      <c r="B193" s="56" t="s">
         <v>522</v>
       </c>
       <c r="C193" s="36" t="s">
@@ -6600,13 +6624,13 @@
       <c r="A194" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="B194" s="32" t="s">
+      <c r="B194" s="68" t="s">
         <v>526</v>
       </c>
-      <c r="C194" s="36" t="s">
+      <c r="C194" s="74" t="s">
         <v>527</v>
       </c>
-      <c r="D194" s="34" t="s">
+      <c r="D194" s="69" t="s">
         <v>528</v>
       </c>
     </row>
@@ -6626,11 +6650,11 @@
       <c r="A196" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="B196" s="32"/>
-      <c r="C196" s="53" t="s">
+      <c r="B196" s="68"/>
+      <c r="C196" s="75" t="s">
         <v>533</v>
       </c>
-      <c r="D196" s="34" t="s">
+      <c r="D196" s="69" t="s">
         <v>534</v>
       </c>
     </row>
@@ -6650,11 +6674,11 @@
       <c r="A198" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="B198" s="32"/>
-      <c r="C198" s="36" t="s">
+      <c r="B198" s="68"/>
+      <c r="C198" s="74" t="s">
         <v>539</v>
       </c>
-      <c r="D198" s="34" t="s">
+      <c r="D198" s="69" t="s">
         <v>540</v>
       </c>
     </row>
@@ -6725,7 +6749,7 @@
       <c r="B204" s="32" t="s">
         <v>978</v>
       </c>
-      <c r="C204" s="54" t="s">
+      <c r="C204" s="53" t="s">
         <v>970</v>
       </c>
       <c r="D204" s="34" t="s">
@@ -6753,10 +6777,10 @@
       <c r="B206" s="32" t="s">
         <v>980</v>
       </c>
-      <c r="C206" s="55" t="s">
+      <c r="C206" s="54" t="s">
         <v>974</v>
       </c>
-      <c r="D206" s="56" t="s">
+      <c r="D206" s="55" t="s">
         <v>975</v>
       </c>
     </row>
@@ -6890,7 +6914,7 @@
       <c r="A217" s="32" t="s">
         <v>961</v>
       </c>
-      <c r="B217" s="58"/>
+      <c r="B217" s="57"/>
       <c r="C217" s="36" t="s">
         <v>962</v>
       </c>
@@ -6902,7 +6926,7 @@
       <c r="A218" s="30" t="s">
         <v>586</v>
       </c>
-      <c r="B218" s="59"/>
+      <c r="B218" s="58"/>
       <c r="C218" s="41" t="s">
         <v>587</v>
       </c>
@@ -6914,7 +6938,7 @@
       <c r="A219" s="29" t="s">
         <v>589</v>
       </c>
-      <c r="B219" s="59"/>
+      <c r="B219" s="58"/>
       <c r="C219" s="47" t="s">
         <v>590</v>
       </c>
@@ -6926,7 +6950,7 @@
       <c r="A220" s="30" t="s">
         <v>592</v>
       </c>
-      <c r="B220" s="59"/>
+      <c r="B220" s="58"/>
       <c r="C220" s="41" t="s">
         <v>593</v>
       </c>
@@ -6938,7 +6962,7 @@
       <c r="A221" s="29" t="s">
         <v>595</v>
       </c>
-      <c r="B221" s="59"/>
+      <c r="B221" s="58"/>
       <c r="C221" s="41" t="s">
         <v>596</v>
       </c>
@@ -6950,7 +6974,7 @@
       <c r="A222" s="30" t="s">
         <v>598</v>
       </c>
-      <c r="B222" s="59"/>
+      <c r="B222" s="58"/>
       <c r="C222" s="41" t="s">
         <v>599</v>
       </c>
@@ -6962,7 +6986,7 @@
       <c r="A223" s="29" t="s">
         <v>601</v>
       </c>
-      <c r="B223" s="59"/>
+      <c r="B223" s="58"/>
       <c r="C223" s="41" t="s">
         <v>602</v>
       </c>
@@ -6974,7 +6998,7 @@
       <c r="A224" s="30" t="s">
         <v>604</v>
       </c>
-      <c r="B224" s="59"/>
+      <c r="B224" s="58"/>
       <c r="C224" s="47" t="s">
         <v>605</v>
       </c>
@@ -6986,7 +7010,7 @@
       <c r="A225" s="29" t="s">
         <v>607</v>
       </c>
-      <c r="B225" s="57"/>
+      <c r="B225" s="56"/>
       <c r="C225" s="41" t="s">
         <v>608</v>
       </c>
@@ -6998,7 +7022,7 @@
       <c r="A226" s="30" t="s">
         <v>610</v>
       </c>
-      <c r="B226" s="57"/>
+      <c r="B226" s="56"/>
       <c r="C226" s="41" t="s">
         <v>611</v>
       </c>
@@ -7010,7 +7034,7 @@
       <c r="A227" s="29" t="s">
         <v>613</v>
       </c>
-      <c r="B227" s="57"/>
+      <c r="B227" s="56"/>
       <c r="C227" s="47" t="s">
         <v>614</v>
       </c>
@@ -7022,7 +7046,7 @@
       <c r="A228" s="30" t="s">
         <v>616</v>
       </c>
-      <c r="B228" s="57"/>
+      <c r="B228" s="56"/>
       <c r="C228" s="41" t="s">
         <v>617</v>
       </c>
@@ -7034,7 +7058,7 @@
       <c r="A229" s="29" t="s">
         <v>619</v>
       </c>
-      <c r="B229" s="57"/>
+      <c r="B229" s="56"/>
       <c r="C229" s="41" t="s">
         <v>620</v>
       </c>
@@ -7046,7 +7070,7 @@
       <c r="A230" s="30" t="s">
         <v>622</v>
       </c>
-      <c r="B230" s="57"/>
+      <c r="B230" s="56"/>
       <c r="C230" s="41" t="s">
         <v>623</v>
       </c>
@@ -7058,7 +7082,7 @@
       <c r="A231" s="29" t="s">
         <v>625</v>
       </c>
-      <c r="B231" s="57"/>
+      <c r="B231" s="56"/>
       <c r="C231" s="41" t="s">
         <v>626</v>
       </c>
@@ -7070,7 +7094,7 @@
       <c r="A232" s="30" t="s">
         <v>628</v>
       </c>
-      <c r="B232" s="57"/>
+      <c r="B232" s="56"/>
       <c r="C232" s="41" t="s">
         <v>629</v>
       </c>
@@ -7082,7 +7106,7 @@
       <c r="A233" s="29" t="s">
         <v>631</v>
       </c>
-      <c r="B233" s="57"/>
+      <c r="B233" s="56"/>
       <c r="C233" s="39" t="s">
         <v>632</v>
       </c>
@@ -7094,7 +7118,7 @@
       <c r="A234" s="30" t="s">
         <v>634</v>
       </c>
-      <c r="B234" s="57"/>
+      <c r="B234" s="56"/>
       <c r="C234" s="41" t="s">
         <v>635</v>
       </c>
@@ -7106,7 +7130,7 @@
       <c r="A235" s="29" t="s">
         <v>637</v>
       </c>
-      <c r="B235" s="57"/>
+      <c r="B235" s="56"/>
       <c r="C235" s="41" t="s">
         <v>638</v>
       </c>
@@ -7118,7 +7142,7 @@
       <c r="A236" s="30" t="s">
         <v>640</v>
       </c>
-      <c r="B236" s="57"/>
+      <c r="B236" s="56"/>
       <c r="C236" s="39" t="s">
         <v>641</v>
       </c>
@@ -7130,7 +7154,7 @@
       <c r="A237" s="29" t="s">
         <v>643</v>
       </c>
-      <c r="B237" s="57"/>
+      <c r="B237" s="56"/>
       <c r="C237" s="39" t="s">
         <v>644</v>
       </c>
@@ -7142,7 +7166,7 @@
       <c r="A238" s="30" t="s">
         <v>646</v>
       </c>
-      <c r="B238" s="57"/>
+      <c r="B238" s="56"/>
       <c r="C238" s="39" t="s">
         <v>647</v>
       </c>
@@ -7154,7 +7178,7 @@
       <c r="A239" s="29" t="s">
         <v>649</v>
       </c>
-      <c r="B239" s="57"/>
+      <c r="B239" s="56"/>
       <c r="C239" s="39" t="s">
         <v>650</v>
       </c>
@@ -7166,7 +7190,7 @@
       <c r="A240" s="30" t="s">
         <v>652</v>
       </c>
-      <c r="B240" s="57"/>
+      <c r="B240" s="56"/>
       <c r="C240" s="44" t="s">
         <v>653</v>
       </c>
@@ -7178,7 +7202,7 @@
       <c r="A241" s="29" t="s">
         <v>655</v>
       </c>
-      <c r="B241" s="57"/>
+      <c r="B241" s="56"/>
       <c r="C241" s="39" t="s">
         <v>656</v>
       </c>
@@ -8386,6 +8410,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010047F5F31BAC119E48A47C88360B4E277D" ma:contentTypeVersion="16" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a594811bfb88eb73205f730fd641aff2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b99410e8-8a6a-49c6-81e8-d5ade3e7c0f2" xmlns:ns3="2192455f-dd39-46c2-a242-0e30632fa188" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33de6fe5c360230ed021394b19300506" ns2:_="" ns3:_="">
     <xsd:import namespace="b99410e8-8a6a-49c6-81e8-d5ade3e7c0f2"/>
@@ -8628,15 +8661,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -8649,6 +8673,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{660C4075-FD93-47A1-BC33-7352171551C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BBC0FCF-CA6B-43B2-840D-46D9480CED33}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8663,14 +8695,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{660C4075-FD93-47A1-BC33-7352171551C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>